<commit_message>
Register user en proceso
</commit_message>
<xml_diff>
--- a/Diagrama.xlsx
+++ b/Diagrama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msancvil\Documents\NTTDATA-UTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA665B7-20E8-4234-8B21-B5B4805AE297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B450E0-D5C3-4A5A-85C6-30C104D5183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{38C96352-42E1-4AFB-A3B4-1F1EF98700B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{38C96352-42E1-4AFB-A3B4-1F1EF98700B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Gant" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>QuestionEspanish</t>
   </si>
   <si>
-    <t>syllabus      [</t>
-  </si>
-  <si>
     <t>Questionnaire        [</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>* Si se cambia la configuracion de los archivos en comun avisar anteriormente y despues del commit, ejemplo Index.JS, package.json</t>
+  </si>
+  <si>
+    <t>Questionnaire  [</t>
   </si>
 </sst>
 </file>
@@ -425,30 +425,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,9 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,266 +813,291 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271890F2-3549-4E8B-B367-EC565FB76558}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="18" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A14:N14"/>
     <mergeCell ref="A1:O3"/>
     <mergeCell ref="A4:B4"/>
@@ -1089,31 +1114,6 @@
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1124,14 +1124,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA01234-852B-4E54-ADB6-1D7A976709DE}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="3.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
     <col min="4" max="4" width="3.08984375" customWidth="1"/>
     <col min="6" max="6" width="2.6328125" customWidth="1"/>
     <col min="7" max="7" width="3.08984375" customWidth="1"/>
@@ -1141,18 +1141,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1160,16 +1160,16 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1177,16 +1177,16 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1194,20 +1194,20 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -1316,7 +1316,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
@@ -1341,7 +1341,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>

</xml_diff>

<commit_message>
Refresh token en proceso
</commit_message>
<xml_diff>
--- a/Diagrama.xlsx
+++ b/Diagrama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msancvil\Documents\NTTDATA-UTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B450E0-D5C3-4A5A-85C6-30C104D5183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671EDC2A-FC0E-4503-90C4-6BC75CE8374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{38C96352-42E1-4AFB-A3B4-1F1EF98700B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{38C96352-42E1-4AFB-A3B4-1F1EF98700B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Gant" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>API DIAGRAMA DE GANT</t>
   </si>
@@ -74,9 +74,6 @@
     <t>LOGIN</t>
   </si>
   <si>
-    <t>REGISTRO</t>
-  </si>
-  <si>
     <t>ESTADO</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Questionnaire  [</t>
+  </si>
+  <si>
+    <t>REGISTER</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +267,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -425,6 +431,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,18 +458,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,6 +502,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,291 +822,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271890F2-3549-4E8B-B367-EC565FB76558}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:N14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A14:N14"/>
     <mergeCell ref="A1:O3"/>
     <mergeCell ref="A4:B4"/>
@@ -1114,6 +1100,31 @@
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1124,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA01234-852B-4E54-ADB6-1D7A976709DE}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1142,7 +1153,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -1202,7 +1213,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -1211,14 +1222,14 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -1228,14 +1239,14 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="10"/>
       <c r="G6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1245,14 +1256,14 @@
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
@@ -1261,14 +1272,14 @@
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
@@ -1277,14 +1288,14 @@
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
@@ -1293,14 +1304,14 @@
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
@@ -1309,14 +1320,14 @@
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
@@ -1325,7 +1336,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -1333,7 +1344,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="12"/>
     </row>
@@ -1341,7 +1352,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
@@ -1350,7 +1361,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -1358,7 +1369,7 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="10"/>
@@ -1366,7 +1377,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -1375,13 +1386,13 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J15" s="12"/>
     </row>
@@ -1391,13 +1402,13 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" s="12"/>
     </row>
@@ -1406,7 +1417,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="10"/>
@@ -1414,7 +1425,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1422,7 +1433,7 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="10"/>
@@ -1430,7 +1441,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1439,13 +1450,13 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="12"/>
     </row>
@@ -1455,7 +1466,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -1468,13 +1479,13 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
@@ -1483,13 +1494,13 @@
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -1498,13 +1509,13 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -1513,7 +1524,7 @@
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>

</xml_diff>

<commit_message>
logout terminado y register en proceso
</commit_message>
<xml_diff>
--- a/Diagrama.xlsx
+++ b/Diagrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msancvil\Documents\NTTDATA-UTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671EDC2A-FC0E-4503-90C4-6BC75CE8374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068418FC-742F-4DCB-A446-1E114CAC68F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{38C96352-42E1-4AFB-A3B4-1F1EF98700B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>API DIAGRAMA DE GANT</t>
   </si>
@@ -77,9 +77,6 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>INFO DEL USUARIO</t>
-  </si>
-  <si>
     <t>ESTRUCTURA MONGO BD</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>REGISTER</t>
+  </si>
+  <si>
+    <t>LOGOUT</t>
   </si>
 </sst>
 </file>
@@ -431,32 +431,35 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,9 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,267 +823,294 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:H6"/>
+      <selection activeCell="I12" sqref="I12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="18" t="s">
+      <c r="A5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A14:N14"/>
     <mergeCell ref="A1:O3"/>
     <mergeCell ref="A4:B4"/>
@@ -1100,31 +1127,6 @@
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1152,18 +1154,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1171,16 +1173,16 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1188,16 +1190,16 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="40"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1205,31 +1207,31 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -1239,14 +1241,14 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="10"/>
       <c r="G6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1256,14 +1258,14 @@
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
@@ -1272,14 +1274,14 @@
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
@@ -1288,14 +1290,14 @@
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
@@ -1304,14 +1306,14 @@
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
@@ -1320,14 +1322,14 @@
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
@@ -1336,7 +1338,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -1344,7 +1346,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" s="12"/>
     </row>
@@ -1352,7 +1354,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
@@ -1361,7 +1363,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -1369,7 +1371,7 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="10"/>
@@ -1377,7 +1379,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -1386,13 +1388,13 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J15" s="12"/>
     </row>
@@ -1402,13 +1404,13 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J16" s="12"/>
     </row>
@@ -1417,7 +1419,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="10"/>
@@ -1425,7 +1427,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1433,7 +1435,7 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="10"/>
@@ -1441,7 +1443,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1450,13 +1452,13 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J19" s="12"/>
     </row>
@@ -1466,7 +1468,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -1479,13 +1481,13 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
@@ -1494,13 +1496,13 @@
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -1509,13 +1511,13 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -1524,7 +1526,7 @@
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>

</xml_diff>